<commit_message>
commiting the entire project including excellib.java file
</commit_message>
<xml_diff>
--- a/src/test/resources/acti/testdata/actidata1.xlsx
+++ b/src/test/resources/acti/testdata/actidata1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Batch20\com.qa.actiTime\src\test\resources\acti\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shobh\git\actitime.automation\src\test\resources\acti\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2423F48-1B20-4E26-AC09-8A88A786D6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A79ED3-FC5B-4B75-9BF0-F0D824798D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,7 +351,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>